<commit_message>
dodanie worda z magisterką gdzie pisze na bierząco, update kosztorysu, nowe bordy
</commit_message>
<xml_diff>
--- a/kosztorys.xlsx
+++ b/kosztorys.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
   <si>
     <t>Silnik krokowy 2</t>
   </si>
@@ -100,6 +100,20 @@
   </si>
   <si>
     <t>dławik drutowy 4u7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N-Mosfet 20V
+P-Mosfet 20V
+68n/50V 
+47n/50
+fotorezystor LDR07 50kR
+rezystor pomiarowy 0R1
+dławik drutowy 20u
+tranzystor PNP
+</t>
+  </si>
+  <si>
+    <t>12.10.14</t>
   </si>
 </sst>
 </file>
@@ -145,9 +159,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -452,7 +469,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -627,20 +644,31 @@
         <v>15</v>
       </c>
     </row>
+    <row r="16" spans="1:5" ht="134.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16">
+        <v>25</v>
+      </c>
+      <c r="E16" t="s">
+        <v>29</v>
+      </c>
+    </row>
     <row r="23" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>4</v>
       </c>
       <c r="C23">
         <f>SUM(C1:C21)</f>
-        <v>366.29999999999995</v>
+        <v>391.29999999999995</v>
       </c>
       <c r="E23" t="s">
         <v>5</v>
       </c>
       <c r="F23" s="1">
         <f>C23/2</f>
-        <v>183.14999999999998</v>
+        <v>195.64999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>